<commit_message>
[DSC-1698] - Refactoring of BulkImportFileUtil (REST)
</commit_message>
<xml_diff>
--- a/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
+++ b/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
@@ -187,25 +187,7 @@
     <t xml:space="preserve">ADDITIONAL-ACCESS-CONDITION</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">file://test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.txt</t>
-    </r>
+    <t xml:space="preserve">file://../bulk-uploads/test.txt</t>
   </si>
   <si>
     <t xml:space="preserve">ORIGINAL</t>
@@ -345,7 +327,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.41"/>
@@ -512,8 +494,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -532,7 +514,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.82"/>
@@ -563,8 +545,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -583,7 +565,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="92.38"/>
@@ -611,8 +593,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -628,10 +610,10 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
@@ -704,14 +686,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="file://test"/>
+    <hyperlink ref="B2" r:id="rId1" display="file://../bulk-uploads/test.txt"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[DSC-1698] Reverts unchanged xls files
</commit_message>
<xml_diff>
--- a/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
+++ b/dspace-api/src/test/data/dspaceFolder/assetstore/bulk-import/items-with-bitstreams.xlsx
@@ -187,7 +187,25 @@
     <t xml:space="preserve">ADDITIONAL-ACCESS-CONDITION</t>
   </si>
   <si>
-    <t xml:space="preserve">file://../bulk-uploads/test.txt</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">file://test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.txt</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ORIGINAL</t>
@@ -327,7 +345,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.41"/>
@@ -494,8 +512,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -514,7 +532,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="81.82"/>
@@ -545,8 +563,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -565,7 +583,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="92.38"/>
@@ -593,8 +611,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -610,10 +628,10 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
@@ -686,14 +704,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="file://../bulk-uploads/test.txt"/>
+    <hyperlink ref="B2" r:id="rId1" display="file://test"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normale"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normale"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>